<commit_message>
:beetle: pandas behaving differently on server
</commit_message>
<xml_diff>
--- a/demo/AcevedoRocha_p450_conversion.xlsx
+++ b/demo/AcevedoRocha_p450_conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteo/Coding/Epistasis_Calculator/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CBB0D9-E9F5-E144-991A-FB2107C53E67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E0B22F-CC08-7B42-BB20-7EFE4BC65E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="2240" windowWidth="24480" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4320" yWindow="2240" windowWidth="24480" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_name" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>Replicate n°1</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Replicate n°3</t>
   </si>
   <si>
-    <t>Mutant 1</t>
-  </si>
-  <si>
     <t>Mutant 2</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>Mutant 7</t>
   </si>
   <si>
-    <t>Mutant 8</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -68,6 +62,15 @@
   </si>
   <si>
     <t>Y51I</t>
+  </si>
+  <si>
+    <t>variant</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>Triple</t>
   </si>
 </sst>
 </file>
@@ -480,21 +483,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -508,16 +512,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>40.408327</v>
@@ -531,16 +535,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>37.383186000000002</v>
@@ -554,16 +558,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>34.551186000000001</v>
@@ -577,16 +581,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>43.913043999999999</v>
@@ -600,16 +604,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>31.102137999999997</v>
@@ -623,16 +627,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>29.781909999999996</v>
@@ -646,16 +650,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>79.956977999999992</v>
@@ -669,16 +673,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>76.937329000000005</v>

</xml_diff>